<commit_message>
Fixed NoneType issue due to empty cells
</commit_message>
<xml_diff>
--- a/contact_list.xlsx
+++ b/contact_list.xlsx
@@ -11,9 +11,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
-  <si>
-    <t>Device</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+  <si>
+    <t>ID</t>
   </si>
   <si>
     <t>First Name</t>
@@ -136,9 +136,6 @@
     <t>Start 5</t>
   </si>
   <si>
-    <t>End 5</t>
-  </si>
-  <si>
     <t>Start 6</t>
   </si>
   <si>
@@ -155,9 +152,6 @@
   </si>
   <si>
     <t>End 8</t>
-  </si>
-  <si>
-    <t>Start 9</t>
   </si>
   <si>
     <t>End 9</t>
@@ -790,19 +784,16 @@
       <c r="B20" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="D20" s="3">
         <v>111.0</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="D21" s="3">
         <v>223.0</v>
@@ -810,10 +801,10 @@
     </row>
     <row r="22">
       <c r="B22" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="D22" s="3">
         <v>165546.0</v>
@@ -821,21 +812,18 @@
     </row>
     <row r="23">
       <c r="B23" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="D23" s="3">
         <v>35.0</v>
       </c>
     </row>
     <row r="24">
-      <c r="B24" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="C24" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D24" s="3">
         <v>1321.0</v>
@@ -843,10 +831,10 @@
     </row>
     <row r="25">
       <c r="B25" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D25" s="3">
         <v>3215498.0</v>
@@ -854,10 +842,10 @@
     </row>
     <row r="26">
       <c r="B26" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D26" s="3">
         <v>849948.0</v>
@@ -865,21 +853,18 @@
     </row>
     <row r="27">
       <c r="B27" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="3">
-        <v>456561.0</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D28" s="3">
         <v>1615615.0</v>
@@ -887,10 +872,10 @@
     </row>
     <row r="29">
       <c r="B29" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D29" s="3">
         <v>661156.0</v>
@@ -901,10 +886,10 @@
         <v>11.0</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D30" s="3">
         <v>99999.0</v>
@@ -912,10 +897,10 @@
     </row>
     <row r="31">
       <c r="B31" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D31" s="3">
         <v>8888.0</v>
@@ -923,10 +908,10 @@
     </row>
     <row r="32">
       <c r="B32" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D32" s="3">
         <v>77777.0</v>
@@ -934,10 +919,10 @@
     </row>
     <row r="33">
       <c r="B33" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D33" s="3">
         <v>99987.0</v>
@@ -945,10 +930,10 @@
     </row>
     <row r="34">
       <c r="B34" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D34" s="3">
         <v>5646541.0</v>
@@ -956,10 +941,10 @@
     </row>
     <row r="35">
       <c r="B35" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D35" s="3">
         <v>123123.0</v>
@@ -967,10 +952,10 @@
     </row>
     <row r="36">
       <c r="B36" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D36" s="3">
         <v>2121.0</v>
@@ -978,10 +963,10 @@
     </row>
     <row r="37">
       <c r="B37" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D37" s="3">
         <v>51050.0</v>
@@ -989,10 +974,10 @@
     </row>
     <row r="38">
       <c r="B38" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D38" s="3">
         <v>2050.0</v>
@@ -1000,10 +985,10 @@
     </row>
     <row r="39">
       <c r="B39" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D39" s="3">
         <v>6060.0</v>
@@ -1011,10 +996,10 @@
     </row>
     <row r="40">
       <c r="B40" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D40" s="3">
         <v>808049.0</v>
@@ -1022,10 +1007,10 @@
     </row>
     <row r="41">
       <c r="B41" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D41" s="3">
         <v>6.5045564E8</v>
@@ -1033,10 +1018,10 @@
     </row>
     <row r="42">
       <c r="B42" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D42" s="3">
         <v>65050.0</v>
@@ -1044,10 +1029,10 @@
     </row>
     <row r="43">
       <c r="B43" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D43" s="3">
         <v>56064.0</v>

</xml_diff>